<commit_message>
Added "ShareSkills" page in Test Excel.
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestData.xlsx
+++ b/MarsFramework/ExcelData/TestData.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19100" windowHeight="7680" activeTab="1"/>
+    <workbookView windowWidth="19100" windowHeight="7680" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp" sheetId="3" r:id="rId1"/>
     <sheet name="SignIn" sheetId="1" r:id="rId2"/>
     <sheet name="Profile" sheetId="2" r:id="rId3"/>
+    <sheet name="ShareSkills" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60">
   <si>
     <t>FirstName</t>
   </si>
@@ -133,6 +134,69 @@
   </si>
   <si>
     <t>kl</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>EnterDescription</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>subcategory</t>
+  </si>
+  <si>
+    <t>TagName</t>
+  </si>
+  <si>
+    <t>ServiceType</t>
+  </si>
+  <si>
+    <t>SelectLocationType</t>
+  </si>
+  <si>
+    <t>SelectSkillTrade</t>
+  </si>
+  <si>
+    <t>UserStatus</t>
+  </si>
+  <si>
+    <t>SaveOrCancel</t>
+  </si>
+  <si>
+    <t>ExchangeSkill</t>
+  </si>
+  <si>
+    <t>AmountInExchange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing </t>
+  </si>
+  <si>
+    <t>I am a Selenium Expert. Would love to share my knowledge.</t>
+  </si>
+  <si>
+    <t>Graphics &amp; Design</t>
+  </si>
+  <si>
+    <t>Book &amp; Album covers</t>
+  </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
+    <t>Hourly basis service</t>
+  </si>
+  <si>
+    <t>On-site</t>
+  </si>
+  <si>
+    <t>Skill-exchange</t>
+  </si>
+  <si>
+    <t>Active</t>
   </si>
 </sst>
 </file>
@@ -140,10 +204,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -165,6 +229,104 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -175,82 +337,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -259,45 +345,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -318,181 +382,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -507,31 +571,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -560,6 +609,45 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -574,39 +662,15 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -624,139 +688,138 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1167,7 +1230,7 @@
   <sheetPr/>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -1193,7 +1256,7 @@
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C2" t="s">
@@ -1204,7 +1267,7 @@
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1231,7 +1294,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2"/>
@@ -1328,4 +1391,111 @@
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="23.5454545454545" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="24.2727272727273" customWidth="1"/>
+    <col min="5" max="5" width="25.3636363636364" customWidth="1"/>
+    <col min="6" max="6" width="25.1818181818182" customWidth="1"/>
+    <col min="7" max="7" width="28.3636363636364" customWidth="1"/>
+    <col min="8" max="8" width="22.2727272727273" customWidth="1"/>
+    <col min="9" max="9" width="18.7272727272727" customWidth="1"/>
+    <col min="10" max="10" width="20" customWidth="1"/>
+    <col min="11" max="11" width="22.4545454545455" customWidth="1"/>
+    <col min="12" max="12" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:12">
+      <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" t="s">
+        <v>55</v>
+      </c>
+      <c r="L2">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>